<commit_message>
Created chapter 4 and updated progress
</commit_message>
<xml_diff>
--- a/01Beginner/Progress.xlsx
+++ b/01Beginner/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Keshav\Programming Languages\Cpp\01Beginner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FBC5B6-F480-4F32-9CDA-63A4EB42E583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C493AA-A76C-48C5-A510-E47607F16CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1D7EFE56-4C4D-4E49-896D-6DD59DD1CFE9}"/>
   </bookViews>
@@ -304,7 +304,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -332,6 +332,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -648,7 +658,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,17 +804,17 @@
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" ref="C5:C20" si="2">IF(F5=1,"Yes",IF(F5&gt;0,"In progress","No"))</f>
-        <v>No</v>
+        <v>In progress</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E5" s="3">
         <v>38</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.31578947368421051</v>
       </c>
       <c r="G5" s="3">
         <v>2</v>
@@ -1292,7 +1302,7 @@
       </c>
       <c r="D21" s="6">
         <f>SUM(D2:D20)</f>
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="E21" s="2">
         <f>SUM(E2:E20)</f>
@@ -1300,7 +1310,7 @@
       </c>
       <c r="F21" s="7">
         <f>D21/E21</f>
-        <v>0.14303959131545338</v>
+        <v>0.15836526181353769</v>
       </c>
       <c r="G21" s="2">
         <f>SUM(G2:G20)</f>
@@ -1333,10 +1343,26 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100248D7B54C96D08408D103F54B92C860E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="89bca6ae96caead7d21ff3eb7eafa021">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c7d20ddf-854b-41ed-ad12-279ea729a3eb" xmlns:ns4="e169787a-ba43-4cf5-82e5-6d4f2fdd5eff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed805198cbcfe4fc26dd4010b744ab5a" ns3:_="" ns4:_="">
     <xsd:import namespace="c7d20ddf-854b-41ed-ad12-279ea729a3eb"/>
@@ -1547,22 +1573,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21C95FC4-7708-40D7-B425-28AC36E5E692}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c7d20ddf-854b-41ed-ad12-279ea729a3eb"/>
+    <ds:schemaRef ds:uri="e169787a-ba43-4cf5-82e5-6d4f2fdd5eff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3F1AE93-8085-415D-8FE9-EA1DE0B2AC69}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A3D5D75-81C7-4BBF-BF55-BF009A8C7BC0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1579,29 +1615,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3F1AE93-8085-415D-8FE9-EA1DE0B2AC69}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21C95FC4-7708-40D7-B425-28AC36E5E692}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c7d20ddf-854b-41ed-ad12-279ea729a3eb"/>
-    <ds:schemaRef ds:uri="e169787a-ba43-4cf5-82e5-6d4f2fdd5eff"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Finished Chapter 5 and Updated Progress xlsx
</commit_message>
<xml_diff>
--- a/01Beginner/Progress.xlsx
+++ b/01Beginner/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Keshav\Programming Languages\Cpp\01Beginner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F83D4E-CA78-4D7C-8F62-F7C71BE20370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1105B8-3BF0-400D-806E-82F9D724379C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1D7EFE56-4C4D-4E49-896D-6DD59DD1CFE9}"/>
   </bookViews>
@@ -54,12 +54,6 @@
     <t># of Day(s)</t>
   </si>
   <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
     <t>Getting Started</t>
   </si>
   <si>
@@ -121,12 +115,21 @@
   </si>
   <si>
     <t>Chapter Completed?</t>
+  </si>
+  <si>
+    <t>Start Date (DD/MM/YYYY)</t>
+  </si>
+  <si>
+    <t>End Date (DD/MM/YYYY)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -207,10 +210,10 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,7 +563,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I19"/>
+      <selection activeCell="G6" sqref="G6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +586,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -598,20 +601,20 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+        <v>27</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="str">
         <f t="shared" ref="C2:C3" si="0">IF(F2=1,"Yes",IF(F2&gt;0,"In progress","No"))</f>
@@ -630,23 +633,22 @@
       <c r="G2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" s="8">
-        <f ca="1">TODAY()</f>
-        <v>44417</v>
-      </c>
-      <c r="I2" s="8">
-        <f ca="1">H2+G2</f>
-        <v>44418</v>
-      </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="H2" s="10">
+        <v>44413</v>
+      </c>
+      <c r="I2" s="10">
+        <f t="shared" ref="I2:I4" si="1">H2+G2-1</f>
+        <v>44413</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="str">
         <f t="shared" si="0"/>
@@ -659,29 +661,29 @@
         <v>42</v>
       </c>
       <c r="F3" s="4">
-        <f t="shared" ref="F3:F20" si="1">D3/E3</f>
+        <f t="shared" ref="F3:F20" si="2">D3/E3</f>
         <v>1</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
       </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H5" ca="1" si="2">TODAY()</f>
-        <v>44417</v>
-      </c>
-      <c r="I3" s="8">
-        <f ca="1">I2</f>
-        <v>44418</v>
-      </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="H3" s="10">
+        <f>I2+1</f>
+        <v>44414</v>
+      </c>
+      <c r="I3" s="10">
+        <f t="shared" si="1"/>
+        <v>44415</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="str">
         <f>IF(F4=1,"Yes",IF(F4&gt;0,"In progress","No"))</f>
@@ -694,32 +696,32 @@
         <v>45</v>
       </c>
       <c r="F4" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G4" s="3">
         <v>2</v>
       </c>
-      <c r="H4" s="8">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H4" s="10">
+        <f>I3+1</f>
+        <v>44416</v>
+      </c>
+      <c r="I4" s="10">
+        <f t="shared" si="1"/>
         <v>44417</v>
       </c>
-      <c r="I4" s="8">
-        <f t="shared" ref="I4" ca="1" si="3">I3</f>
-        <v>44418</v>
-      </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="str">
-        <f t="shared" ref="C5:C20" si="4">IF(F5=1,"Yes",IF(F5&gt;0,"In progress","No"))</f>
+        <f t="shared" ref="C5:C20" si="3">IF(F5=1,"Yes",IF(F5&gt;0,"In progress","No"))</f>
         <v>Yes</v>
       </c>
       <c r="D5" s="3">
@@ -729,67 +731,67 @@
         <v>38</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G5" s="3">
         <v>2</v>
       </c>
-      <c r="H5" s="8">
-        <f t="shared" ca="1" si="2"/>
-        <v>44417</v>
-      </c>
-      <c r="I5" s="8">
-        <f t="shared" ref="I5:I20" ca="1" si="5">H5+G5</f>
+      <c r="H5" s="10">
+        <f>I4+1</f>
+        <v>44418</v>
+      </c>
+      <c r="I5" s="10">
+        <f>H5+G5-1</f>
         <v>44419</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>No</v>
+        <f t="shared" si="3"/>
+        <v>Yes</v>
       </c>
       <c r="D6" s="3">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E6" s="3">
         <v>25</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
       </c>
-      <c r="H6" s="8">
-        <f t="shared" ref="H6:H20" ca="1" si="6">I5+1</f>
+      <c r="H6" s="10">
+        <f t="shared" ref="H6:H20" si="4">I5+1</f>
         <v>44420</v>
       </c>
-      <c r="I6" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44421</v>
-      </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
+      <c r="I6" s="10">
+        <f t="shared" ref="I6:I20" si="5">H6+G6-1</f>
+        <v>44420</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>No</v>
       </c>
       <c r="D7" s="3">
@@ -799,32 +801,32 @@
         <v>56</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G7" s="3">
         <v>3</v>
       </c>
-      <c r="H7" s="8">
-        <f t="shared" ca="1" si="6"/>
-        <v>44422</v>
-      </c>
-      <c r="I7" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44425</v>
-      </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
+      <c r="H7" s="10">
+        <f t="shared" si="4"/>
+        <v>44421</v>
+      </c>
+      <c r="I7" s="10">
+        <f t="shared" si="5"/>
+        <v>44423</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>No</v>
       </c>
       <c r="D8" s="3">
@@ -834,32 +836,32 @@
         <v>58</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G8" s="3">
         <v>3</v>
       </c>
-      <c r="H8" s="8">
-        <f t="shared" ca="1" si="6"/>
+      <c r="H8" s="10">
+        <f t="shared" si="4"/>
+        <v>44424</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="5"/>
         <v>44426</v>
       </c>
-      <c r="I8" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44429</v>
-      </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>No</v>
       </c>
       <c r="D9" s="3">
@@ -869,32 +871,32 @@
         <v>14</v>
       </c>
       <c r="F9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
       </c>
-      <c r="H9" s="8">
-        <f t="shared" ca="1" si="6"/>
-        <v>44430</v>
-      </c>
-      <c r="I9" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44431</v>
-      </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
+      <c r="H9" s="10">
+        <f t="shared" si="4"/>
+        <v>44427</v>
+      </c>
+      <c r="I9" s="10">
+        <f t="shared" si="5"/>
+        <v>44427</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>No</v>
       </c>
       <c r="D10" s="3">
@@ -904,32 +906,32 @@
         <v>52</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G10" s="3">
         <v>3</v>
       </c>
-      <c r="H10" s="8">
-        <f t="shared" ca="1" si="6"/>
-        <v>44432</v>
-      </c>
-      <c r="I10" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44435</v>
-      </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="H10" s="10">
+        <f t="shared" si="4"/>
+        <v>44428</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="5"/>
+        <v>44430</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>No</v>
       </c>
       <c r="D11" s="3">
@@ -939,32 +941,32 @@
         <v>42</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G11" s="3">
         <v>2</v>
       </c>
-      <c r="H11" s="8">
-        <f t="shared" ca="1" si="6"/>
-        <v>44436</v>
-      </c>
-      <c r="I11" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44438</v>
-      </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
+      <c r="H11" s="10">
+        <f t="shared" si="4"/>
+        <v>44431</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="5"/>
+        <v>44432</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>No</v>
       </c>
       <c r="D12" s="3">
@@ -974,32 +976,32 @@
         <v>38</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G12" s="3">
         <v>2</v>
       </c>
-      <c r="H12" s="8">
-        <f t="shared" ca="1" si="6"/>
-        <v>44439</v>
-      </c>
-      <c r="I12" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44441</v>
-      </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
+      <c r="H12" s="10">
+        <f t="shared" si="4"/>
+        <v>44433</v>
+      </c>
+      <c r="I12" s="10">
+        <f t="shared" si="5"/>
+        <v>44434</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>No</v>
       </c>
       <c r="D13" s="3">
@@ -1009,32 +1011,32 @@
         <v>33</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G13" s="3">
         <v>2</v>
       </c>
-      <c r="H13" s="8">
-        <f t="shared" ca="1" si="6"/>
-        <v>44442</v>
-      </c>
-      <c r="I13" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44444</v>
-      </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
+      <c r="H13" s="10">
+        <f t="shared" si="4"/>
+        <v>44435</v>
+      </c>
+      <c r="I13" s="10">
+        <f t="shared" si="5"/>
+        <v>44436</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>No</v>
       </c>
       <c r="D14" s="3">
@@ -1044,32 +1046,32 @@
         <v>58</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G14" s="3">
         <v>3</v>
       </c>
-      <c r="H14" s="8">
-        <f t="shared" ca="1" si="6"/>
-        <v>44445</v>
-      </c>
-      <c r="I14" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44448</v>
-      </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
+      <c r="H14" s="10">
+        <f t="shared" si="4"/>
+        <v>44437</v>
+      </c>
+      <c r="I14" s="10">
+        <f t="shared" si="5"/>
+        <v>44439</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>No</v>
       </c>
       <c r="D15" s="3">
@@ -1079,32 +1081,32 @@
         <v>53</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G15" s="3">
         <v>3</v>
       </c>
-      <c r="H15" s="8">
-        <f t="shared" ca="1" si="6"/>
-        <v>44449</v>
-      </c>
-      <c r="I15" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44452</v>
-      </c>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
+      <c r="H15" s="10">
+        <f t="shared" si="4"/>
+        <v>44440</v>
+      </c>
+      <c r="I15" s="10">
+        <f t="shared" si="5"/>
+        <v>44442</v>
+      </c>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>No</v>
       </c>
       <c r="D16" s="3">
@@ -1114,32 +1116,32 @@
         <v>42</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G16" s="3">
         <v>2</v>
       </c>
-      <c r="H16" s="8">
-        <f t="shared" ca="1" si="6"/>
-        <v>44453</v>
-      </c>
-      <c r="I16" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44455</v>
-      </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
+      <c r="H16" s="10">
+        <f t="shared" si="4"/>
+        <v>44443</v>
+      </c>
+      <c r="I16" s="10">
+        <f t="shared" si="5"/>
+        <v>44444</v>
+      </c>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>No</v>
       </c>
       <c r="D17" s="3">
@@ -1149,32 +1151,32 @@
         <v>67</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G17" s="3">
         <v>3</v>
       </c>
-      <c r="H17" s="8">
-        <f t="shared" ca="1" si="6"/>
-        <v>44456</v>
-      </c>
-      <c r="I17" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44459</v>
-      </c>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
+      <c r="H17" s="10">
+        <f t="shared" si="4"/>
+        <v>44445</v>
+      </c>
+      <c r="I17" s="10">
+        <f t="shared" si="5"/>
+        <v>44447</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>No</v>
       </c>
       <c r="D18" s="3">
@@ -1184,32 +1186,32 @@
         <v>39</v>
       </c>
       <c r="F18" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G18" s="3">
         <v>2</v>
       </c>
-      <c r="H18" s="8">
-        <f t="shared" ca="1" si="6"/>
-        <v>44460</v>
-      </c>
-      <c r="I18" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44462</v>
-      </c>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
+      <c r="H18" s="10">
+        <f t="shared" si="4"/>
+        <v>44448</v>
+      </c>
+      <c r="I18" s="10">
+        <f t="shared" si="5"/>
+        <v>44449</v>
+      </c>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>No</v>
       </c>
       <c r="D19" s="3">
@@ -1219,19 +1221,19 @@
         <v>30</v>
       </c>
       <c r="F19" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G19" s="3">
         <v>2</v>
       </c>
-      <c r="H19" s="8">
-        <f t="shared" ca="1" si="6"/>
-        <v>44463</v>
-      </c>
-      <c r="I19" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44465</v>
+      <c r="H19" s="10">
+        <f t="shared" si="4"/>
+        <v>44450</v>
+      </c>
+      <c r="I19" s="10">
+        <f t="shared" si="5"/>
+        <v>44451</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1239,10 +1241,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>No</v>
       </c>
       <c r="D20" s="3">
@@ -1252,33 +1254,33 @@
         <v>26</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G20" s="3">
         <v>1</v>
       </c>
-      <c r="H20" s="8">
-        <f t="shared" ca="1" si="6"/>
-        <v>44466</v>
-      </c>
-      <c r="I20" s="8">
-        <f t="shared" ca="1" si="5"/>
-        <v>44467</v>
+      <c r="H20" s="10">
+        <f t="shared" si="4"/>
+        <v>44452</v>
+      </c>
+      <c r="I20" s="10">
+        <f t="shared" si="5"/>
+        <v>44452</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="5">
         <f>COUNTIF(C2:C20,"Yes")/19</f>
-        <v>0.21052631578947367</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="D21" s="6">
         <f>SUM(D2:D20)</f>
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="E21" s="2">
         <f>SUM(E2:E20)</f>
@@ -1286,14 +1288,20 @@
       </c>
       <c r="F21" s="7">
         <f>D21/E21</f>
-        <v>0.19157088122605365</v>
+        <v>0.22349936143039592</v>
       </c>
       <c r="G21" s="2">
         <f>SUM(G2:G20)</f>
         <v>40</v>
       </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
+      <c r="H21" s="11">
+        <f>H2</f>
+        <v>44413</v>
+      </c>
+      <c r="I21" s="11">
+        <f>I20</f>
+        <v>44452</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
@@ -1320,6 +1328,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100248D7B54C96D08408D103F54B92C860E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="89bca6ae96caead7d21ff3eb7eafa021">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c7d20ddf-854b-41ed-ad12-279ea729a3eb" xmlns:ns4="e169787a-ba43-4cf5-82e5-6d4f2fdd5eff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed805198cbcfe4fc26dd4010b744ab5a" ns3:_="" ns4:_="">
     <xsd:import namespace="c7d20ddf-854b-41ed-ad12-279ea729a3eb"/>
@@ -1530,22 +1553,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21C95FC4-7708-40D7-B425-28AC36E5E692}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c7d20ddf-854b-41ed-ad12-279ea729a3eb"/>
+    <ds:schemaRef ds:uri="e169787a-ba43-4cf5-82e5-6d4f2fdd5eff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3F1AE93-8085-415D-8FE9-EA1DE0B2AC69}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A3D5D75-81C7-4BBF-BF55-BF009A8C7BC0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1562,29 +1595,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3F1AE93-8085-415D-8FE9-EA1DE0B2AC69}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21C95FC4-7708-40D7-B425-28AC36E5E692}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c7d20ddf-854b-41ed-ad12-279ea729a3eb"/>
-    <ds:schemaRef ds:uri="e169787a-ba43-4cf5-82e5-6d4f2fdd5eff"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Chapter 6 Data
</commit_message>
<xml_diff>
--- a/01Beginner/Progress.xlsx
+++ b/01Beginner/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Keshav\Programming Languages\Cpp\01Beginner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6BB47A-1B24-4AB0-8E13-F4DD5C102571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C5AE84-A1D4-413E-B006-28828FD984EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1D7EFE56-4C4D-4E49-896D-6DD59DD1CFE9}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11505" xr2:uid="{1D7EFE56-4C4D-4E49-896D-6DD59DD1CFE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -575,7 +575,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="D8" sqref="D8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +651,7 @@
         <v>44413</v>
       </c>
       <c r="I2" s="9">
-        <f>H2+G2-1</f>
+        <f t="shared" ref="I2:I20" si="1">H2+G2-1</f>
         <v>44413</v>
       </c>
       <c r="J2" s="13">
@@ -678,7 +678,7 @@
         <v>42</v>
       </c>
       <c r="F3" s="4">
-        <f t="shared" ref="F3:F20" si="1">D3/E3</f>
+        <f t="shared" ref="F3:F20" si="2">D3/E3</f>
         <v>1</v>
       </c>
       <c r="G3" s="3">
@@ -689,11 +689,11 @@
         <v>44414</v>
       </c>
       <c r="I3" s="9">
-        <f>H3+G3-1</f>
+        <f t="shared" si="1"/>
         <v>44415</v>
       </c>
       <c r="J3" s="13">
-        <f t="shared" ref="J3:J20" si="2">IF(C3="Yes",G3,0)</f>
+        <f t="shared" ref="J3:J20" si="3">IF(C3="Yes",G3,0)</f>
         <v>2</v>
       </c>
       <c r="K3" s="8"/>
@@ -716,7 +716,7 @@
         <v>45</v>
       </c>
       <c r="F4" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G4" s="3">
@@ -727,11 +727,11 @@
         <v>44416</v>
       </c>
       <c r="I4" s="9">
-        <f>H4+G4-1</f>
+        <f t="shared" si="1"/>
         <v>44417</v>
       </c>
       <c r="J4" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="K4" s="8"/>
@@ -744,7 +744,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="str">
-        <f t="shared" ref="C5:C20" si="3">IF(F5=1,"Yes",IF(F5&gt;0,"In progress","No"))</f>
+        <f t="shared" ref="C5:C20" si="4">IF(F5=1,"Yes",IF(F5&gt;0,"In progress","No"))</f>
         <v>Yes</v>
       </c>
       <c r="D5" s="3">
@@ -754,7 +754,7 @@
         <v>38</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G5" s="3">
@@ -765,11 +765,11 @@
         <v>44418</v>
       </c>
       <c r="I5" s="9">
-        <f>H5+G5-1</f>
+        <f t="shared" si="1"/>
         <v>44419</v>
       </c>
       <c r="J5" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="K5" s="8"/>
@@ -782,7 +782,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Yes</v>
       </c>
       <c r="D6" s="3">
@@ -792,22 +792,22 @@
         <v>25</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
       </c>
       <c r="H6" s="9">
-        <f t="shared" ref="H6:H20" si="4">I5+1</f>
+        <f t="shared" ref="H6:H20" si="5">I5+1</f>
         <v>44420</v>
       </c>
       <c r="I6" s="9">
-        <f>H6+G6-1</f>
+        <f t="shared" si="1"/>
         <v>44420</v>
       </c>
       <c r="J6" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K6" s="8"/>
@@ -820,33 +820,33 @@
         <v>11</v>
       </c>
       <c r="C7" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>In progress</v>
+        <f t="shared" si="4"/>
+        <v>Yes</v>
       </c>
       <c r="D7" s="3">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="E7" s="3">
         <v>56</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" si="1"/>
-        <v>0.42857142857142855</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="G7" s="3">
         <v>3</v>
       </c>
       <c r="H7" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44421</v>
       </c>
       <c r="I7" s="9">
-        <f>H7+G7-1</f>
+        <f t="shared" si="1"/>
         <v>44423</v>
       </c>
       <c r="J7" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3</v>
       </c>
       <c r="K7" s="8"/>
     </row>
@@ -858,7 +858,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>No</v>
       </c>
       <c r="D8" s="3">
@@ -868,22 +868,22 @@
         <v>58</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G8" s="3">
         <v>3</v>
       </c>
       <c r="H8" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44424</v>
       </c>
       <c r="I8" s="9">
-        <f>H8+G8-1</f>
+        <f t="shared" si="1"/>
         <v>44426</v>
       </c>
       <c r="J8" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K8" s="8"/>
@@ -896,7 +896,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>No</v>
       </c>
       <c r="D9" s="3">
@@ -906,22 +906,22 @@
         <v>14</v>
       </c>
       <c r="F9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
       </c>
       <c r="H9" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44427</v>
       </c>
       <c r="I9" s="9">
-        <f>H9+G9-1</f>
+        <f t="shared" si="1"/>
         <v>44427</v>
       </c>
       <c r="J9" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K9" s="8"/>
@@ -934,7 +934,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>No</v>
       </c>
       <c r="D10" s="3">
@@ -944,22 +944,22 @@
         <v>52</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G10" s="3">
         <v>3</v>
       </c>
       <c r="H10" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44428</v>
       </c>
       <c r="I10" s="9">
-        <f>H10+G10-1</f>
+        <f t="shared" si="1"/>
         <v>44430</v>
       </c>
       <c r="J10" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K10" s="8"/>
@@ -972,7 +972,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>No</v>
       </c>
       <c r="D11" s="3">
@@ -982,22 +982,22 @@
         <v>42</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G11" s="3">
         <v>2</v>
       </c>
       <c r="H11" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44431</v>
       </c>
       <c r="I11" s="9">
-        <f>H11+G11-1</f>
+        <f t="shared" si="1"/>
         <v>44432</v>
       </c>
       <c r="J11" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K11" s="8"/>
@@ -1010,7 +1010,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>No</v>
       </c>
       <c r="D12" s="3">
@@ -1020,22 +1020,22 @@
         <v>38</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G12" s="3">
         <v>2</v>
       </c>
       <c r="H12" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44433</v>
       </c>
       <c r="I12" s="9">
-        <f>H12+G12-1</f>
+        <f t="shared" si="1"/>
         <v>44434</v>
       </c>
       <c r="J12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K12" s="8"/>
@@ -1048,7 +1048,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>No</v>
       </c>
       <c r="D13" s="3">
@@ -1058,22 +1058,22 @@
         <v>33</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G13" s="3">
         <v>2</v>
       </c>
       <c r="H13" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44435</v>
       </c>
       <c r="I13" s="9">
-        <f>H13+G13-1</f>
+        <f t="shared" si="1"/>
         <v>44436</v>
       </c>
       <c r="J13" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K13" s="8"/>
@@ -1086,7 +1086,7 @@
         <v>18</v>
       </c>
       <c r="C14" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>No</v>
       </c>
       <c r="D14" s="3">
@@ -1096,22 +1096,22 @@
         <v>58</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G14" s="3">
         <v>3</v>
       </c>
       <c r="H14" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44437</v>
       </c>
       <c r="I14" s="9">
-        <f>H14+G14-1</f>
+        <f t="shared" si="1"/>
         <v>44439</v>
       </c>
       <c r="J14" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K14" s="8"/>
@@ -1124,7 +1124,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>No</v>
       </c>
       <c r="D15" s="3">
@@ -1134,22 +1134,22 @@
         <v>53</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G15" s="3">
         <v>3</v>
       </c>
       <c r="H15" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44440</v>
       </c>
       <c r="I15" s="9">
-        <f>H15+G15-1</f>
+        <f t="shared" si="1"/>
         <v>44442</v>
       </c>
       <c r="J15" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K15" s="8"/>
@@ -1162,7 +1162,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>No</v>
       </c>
       <c r="D16" s="3">
@@ -1172,22 +1172,22 @@
         <v>42</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G16" s="3">
         <v>2</v>
       </c>
       <c r="H16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44443</v>
       </c>
       <c r="I16" s="9">
-        <f>H16+G16-1</f>
+        <f t="shared" si="1"/>
         <v>44444</v>
       </c>
       <c r="J16" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K16" s="8"/>
@@ -1200,7 +1200,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>No</v>
       </c>
       <c r="D17" s="3">
@@ -1210,22 +1210,22 @@
         <v>67</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G17" s="3">
         <v>3</v>
       </c>
       <c r="H17" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44445</v>
       </c>
       <c r="I17" s="9">
-        <f>H17+G17-1</f>
+        <f t="shared" si="1"/>
         <v>44447</v>
       </c>
       <c r="J17" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K17" s="8"/>
@@ -1238,7 +1238,7 @@
         <v>22</v>
       </c>
       <c r="C18" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>No</v>
       </c>
       <c r="D18" s="3">
@@ -1248,22 +1248,22 @@
         <v>39</v>
       </c>
       <c r="F18" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G18" s="3">
         <v>2</v>
       </c>
       <c r="H18" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44448</v>
       </c>
       <c r="I18" s="9">
-        <f>H18+G18-1</f>
+        <f t="shared" si="1"/>
         <v>44449</v>
       </c>
       <c r="J18" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K18" s="8"/>
@@ -1276,7 +1276,7 @@
         <v>23</v>
       </c>
       <c r="C19" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>No</v>
       </c>
       <c r="D19" s="3">
@@ -1286,22 +1286,22 @@
         <v>30</v>
       </c>
       <c r="F19" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G19" s="3">
         <v>2</v>
       </c>
       <c r="H19" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44450</v>
       </c>
       <c r="I19" s="9">
-        <f>H19+G19-1</f>
+        <f t="shared" si="1"/>
         <v>44451</v>
       </c>
       <c r="J19" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
         <v>24</v>
       </c>
       <c r="C20" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>No</v>
       </c>
       <c r="D20" s="3">
@@ -1323,22 +1323,22 @@
         <v>26</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G20" s="3">
         <v>1</v>
       </c>
       <c r="H20" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44452</v>
       </c>
       <c r="I20" s="9">
-        <f>H20+G20-1</f>
+        <f t="shared" si="1"/>
         <v>44452</v>
       </c>
       <c r="J20" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K20" s="17"/>
@@ -1350,11 +1350,11 @@
       <c r="B21" s="2"/>
       <c r="C21" s="5">
         <f>COUNTIF(C2:C20,"Yes")/19</f>
-        <v>0.26315789473684209</v>
+        <v>0.31578947368421051</v>
       </c>
       <c r="D21" s="6">
         <f>SUM(D2:D20)</f>
-        <v>199</v>
+        <v>231</v>
       </c>
       <c r="E21" s="2">
         <f>SUM(E2:E20)</f>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="F21" s="7">
         <f>D21/E21</f>
-        <v>0.25415070242656451</v>
+        <v>0.2950191570881226</v>
       </c>
       <c r="G21" s="2">
         <f>SUM(G2:G20)</f>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="J22" s="16">
         <f>G21-SUM(J2:J20)</f>
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1413,6 +1413,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100248D7B54C96D08408D103F54B92C860E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="89bca6ae96caead7d21ff3eb7eafa021">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c7d20ddf-854b-41ed-ad12-279ea729a3eb" xmlns:ns4="e169787a-ba43-4cf5-82e5-6d4f2fdd5eff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed805198cbcfe4fc26dd4010b744ab5a" ns3:_="" ns4:_="">
     <xsd:import namespace="c7d20ddf-854b-41ed-ad12-279ea729a3eb"/>
@@ -1623,22 +1638,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21C95FC4-7708-40D7-B425-28AC36E5E692}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c7d20ddf-854b-41ed-ad12-279ea729a3eb"/>
+    <ds:schemaRef ds:uri="e169787a-ba43-4cf5-82e5-6d4f2fdd5eff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3F1AE93-8085-415D-8FE9-EA1DE0B2AC69}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A3D5D75-81C7-4BBF-BF55-BF009A8C7BC0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1655,29 +1680,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3F1AE93-8085-415D-8FE9-EA1DE0B2AC69}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21C95FC4-7708-40D7-B425-28AC36E5E692}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c7d20ddf-854b-41ed-ad12-279ea729a3eb"/>
-    <ds:schemaRef ds:uri="e169787a-ba43-4cf5-82e5-6d4f2fdd5eff"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>